<commit_message>
Ajout commentaire dans les classes Persistance
</commit_message>
<xml_diff>
--- a/TestsSaveExcel/Etalonnage.xlsx
+++ b/TestsSaveExcel/Etalonnage.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Etalonnage" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="NewEtalonnage" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="29">
   <si>
     <t xml:space="preserve">Groupe</t>
   </si>
@@ -87,14 +88,36 @@
   <si>
     <t xml:space="preserve">60-69</t>
   </si>
+  <si>
+    <t xml:space="preserve">Pour ET voir pour faire des paliers pour limiter le nombre de cas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x-/x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(x-/x)²</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moyenne : </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Somme : </t>
+  </si>
+  <si>
+    <t xml:space="preserve">E.T : </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.00"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -128,8 +151,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFCC6600"/>
-        <bgColor rgb="FF808000"/>
+        <fgColor rgb="FF77BC65"/>
+        <bgColor rgb="FF99CC00"/>
       </patternFill>
     </fill>
     <fill>
@@ -292,7 +315,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="48">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -463,6 +486,26 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -521,9 +564,9 @@
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFCC6600"/>
+      <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF77BC65"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
@@ -542,16 +585,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M51"/>
+  <dimension ref="A1:M59"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K14" activeCellId="0" sqref="K14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="1" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="12.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="20.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1791,4 +1836,1428 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:N49"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K13" activeCellId="0" sqref="K13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="2" style="0" width="10.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="20.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="0" width="10.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3"/>
+      <c r="G1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="4"/>
+      <c r="J1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="5" t="str">
+        <f aca="false">CONCATENATE("Stagiaires testés ( ",SUM(K2:K8)," )")</f>
+        <v>Stagiaires testés ( 180 )</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="4"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="1"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="12" t="n">
+        <v>26.3</v>
+      </c>
+      <c r="D3" s="12" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="E3" s="12" t="n">
+        <v>7.6</v>
+      </c>
+      <c r="F3" s="12" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="G3" s="12" t="n">
+        <v>64.5</v>
+      </c>
+      <c r="H3" s="13" t="n">
+        <v>14.8</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="15" t="n">
+        <v>93</v>
+      </c>
+      <c r="L3" s="15" t="n">
+        <v>20</v>
+      </c>
+      <c r="M3" s="16" t="n">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="10"/>
+      <c r="B4" s="17" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="18" t="n">
+        <v>18.5</v>
+      </c>
+      <c r="D4" s="18" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="E4" s="18" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="F4" s="18" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="G4" s="18" t="n">
+        <v>68</v>
+      </c>
+      <c r="H4" s="19" t="n">
+        <v>12.9</v>
+      </c>
+      <c r="J4" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4" s="21" t="n">
+        <v>19</v>
+      </c>
+      <c r="L4" s="21" t="n">
+        <v>35.1</v>
+      </c>
+      <c r="M4" s="22" t="n">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="10"/>
+      <c r="B5" s="23" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" s="24" t="n">
+        <v>15.9</v>
+      </c>
+      <c r="D5" s="24" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="E5" s="24" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="F5" s="24" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="G5" s="24" t="n">
+        <v>77.9</v>
+      </c>
+      <c r="H5" s="25" t="n">
+        <v>12.7</v>
+      </c>
+      <c r="J5" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" s="27" t="n">
+        <v>11</v>
+      </c>
+      <c r="L5" s="27" t="n">
+        <v>44.2</v>
+      </c>
+      <c r="M5" s="28" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="10"/>
+      <c r="B6" s="17" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" s="18" t="n">
+        <v>14.4</v>
+      </c>
+      <c r="D6" s="18" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E6" s="18" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="F6" s="18" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="G6" s="18" t="n">
+        <v>85.7</v>
+      </c>
+      <c r="H6" s="19" t="n">
+        <v>12.7</v>
+      </c>
+      <c r="J6" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" s="21" t="n">
+        <v>10</v>
+      </c>
+      <c r="L6" s="21" t="n">
+        <v>52.6</v>
+      </c>
+      <c r="M6" s="22" t="n">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="10"/>
+      <c r="B7" s="23" t="n">
+        <v>5</v>
+      </c>
+      <c r="C7" s="24" t="n">
+        <v>13.5</v>
+      </c>
+      <c r="D7" s="24" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="E7" s="24" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="F7" s="24" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="G7" s="24" t="n">
+        <v>91.1</v>
+      </c>
+      <c r="H7" s="25" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="J7" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="K7" s="27" t="n">
+        <v>26</v>
+      </c>
+      <c r="L7" s="27" t="n">
+        <v>64.9</v>
+      </c>
+      <c r="M7" s="28" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="10"/>
+      <c r="B8" s="17" t="n">
+        <v>6</v>
+      </c>
+      <c r="C8" s="18" t="n">
+        <v>13.6</v>
+      </c>
+      <c r="D8" s="18" t="n">
+        <v>2</v>
+      </c>
+      <c r="E8" s="18" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F8" s="18" t="n">
+        <v>2</v>
+      </c>
+      <c r="G8" s="18" t="n">
+        <v>90.2</v>
+      </c>
+      <c r="H8" s="19" t="n">
+        <v>10.7</v>
+      </c>
+      <c r="J8" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="K8" s="30" t="n">
+        <v>21</v>
+      </c>
+      <c r="L8" s="30" t="n">
+        <v>74.7</v>
+      </c>
+      <c r="M8" s="31" t="n">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="10"/>
+      <c r="B9" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="33" t="n">
+        <v>17</v>
+      </c>
+      <c r="D9" s="33" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="E9" s="33" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="F9" s="33" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="G9" s="33" t="n">
+        <v>79.6</v>
+      </c>
+      <c r="H9" s="34" t="n">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="35"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="38" t="n">
+        <v>27.6</v>
+      </c>
+      <c r="D11" s="38" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="E11" s="38" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="F11" s="38" t="n">
+        <v>5</v>
+      </c>
+      <c r="G11" s="38" t="n">
+        <v>61.8</v>
+      </c>
+      <c r="H11" s="39" t="n">
+        <v>15.2</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="10"/>
+      <c r="B12" s="23" t="n">
+        <v>2</v>
+      </c>
+      <c r="C12" s="24" t="n">
+        <v>19.4</v>
+      </c>
+      <c r="D12" s="24" t="n">
+        <v>4</v>
+      </c>
+      <c r="E12" s="24" t="n">
+        <v>7.3</v>
+      </c>
+      <c r="F12" s="24" t="n">
+        <v>4</v>
+      </c>
+      <c r="G12" s="24" t="n">
+        <v>64.9</v>
+      </c>
+      <c r="H12" s="25" t="n">
+        <v>13</v>
+      </c>
+      <c r="K12" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="10"/>
+      <c r="B13" s="17" t="n">
+        <v>3</v>
+      </c>
+      <c r="C13" s="18" t="n">
+        <v>17.6</v>
+      </c>
+      <c r="D13" s="18" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="E13" s="18" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="F13" s="18" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="G13" s="18" t="n">
+        <v>74.6</v>
+      </c>
+      <c r="H13" s="19" t="n">
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="10"/>
+      <c r="B14" s="23" t="n">
+        <v>4</v>
+      </c>
+      <c r="C14" s="24" t="n">
+        <v>15.2</v>
+      </c>
+      <c r="D14" s="24" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="E14" s="24" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="F14" s="24" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="G14" s="24" t="n">
+        <v>80.9</v>
+      </c>
+      <c r="H14" s="25" t="n">
+        <v>11.8</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="10"/>
+      <c r="B15" s="17" t="n">
+        <v>5</v>
+      </c>
+      <c r="C15" s="18" t="n">
+        <v>14.4</v>
+      </c>
+      <c r="D15" s="18" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E15" s="18" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="F15" s="18" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="G15" s="18" t="n">
+        <v>84.9</v>
+      </c>
+      <c r="H15" s="19" t="n">
+        <v>10.4</v>
+      </c>
+      <c r="L15" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="M15" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="N15" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="10"/>
+      <c r="B16" s="23" t="n">
+        <v>6</v>
+      </c>
+      <c r="C16" s="24" t="n">
+        <v>14.1</v>
+      </c>
+      <c r="D16" s="24" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="E16" s="24" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="F16" s="24" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G16" s="24" t="n">
+        <v>86.3</v>
+      </c>
+      <c r="H16" s="25" t="n">
+        <v>8.6</v>
+      </c>
+      <c r="K16" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="L16" s="43" t="n">
+        <v>4</v>
+      </c>
+      <c r="M16" s="44" t="n">
+        <f aca="false">IF(L16 = "",,(L16-$L$26))</f>
+        <v>-2.5</v>
+      </c>
+      <c r="N16" s="44" t="n">
+        <f aca="false">IF(L16 = "",,POWER((L16-$L$26),2))</f>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="10"/>
+      <c r="B17" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="41" t="n">
+        <v>18</v>
+      </c>
+      <c r="D17" s="41" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="E17" s="41" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="F17" s="41" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="G17" s="41" t="n">
+        <v>75.6</v>
+      </c>
+      <c r="H17" s="42" t="n">
+        <v>10</v>
+      </c>
+      <c r="K17" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="L17" s="43" t="n">
+        <v>6</v>
+      </c>
+      <c r="M17" s="44" t="n">
+        <f aca="false">IF(L17 = "",,(L17-$L$26))</f>
+        <v>-0.5</v>
+      </c>
+      <c r="N17" s="44" t="n">
+        <f aca="false">IF(L17 = "",,POWER((L17-$L$26),2))</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
+      <c r="K18" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="L18" s="43" t="n">
+        <v>8</v>
+      </c>
+      <c r="M18" s="44" t="n">
+        <f aca="false">IF(L18 = "",,(L18-$L$26))</f>
+        <v>1.5</v>
+      </c>
+      <c r="N18" s="44" t="n">
+        <f aca="false">IF(L18 = "",,POWER((L18-$L$26),2))</f>
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" s="12" t="n">
+        <v>27.4</v>
+      </c>
+      <c r="D19" s="12" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="E19" s="12" t="n">
+        <v>6.9</v>
+      </c>
+      <c r="F19" s="12" t="n">
+        <v>4</v>
+      </c>
+      <c r="G19" s="12" t="n">
+        <v>66.4</v>
+      </c>
+      <c r="H19" s="13" t="n">
+        <v>14.6</v>
+      </c>
+      <c r="K19" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="L19" s="43" t="n">
+        <v>10</v>
+      </c>
+      <c r="M19" s="44" t="n">
+        <f aca="false">IF(L19 = "",,(L19-$L$26))</f>
+        <v>3.5</v>
+      </c>
+      <c r="N19" s="44" t="n">
+        <f aca="false">IF(L19 = "",,POWER((L19-$L$26),2))</f>
+        <v>12.25</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="10"/>
+      <c r="B20" s="17" t="n">
+        <v>2</v>
+      </c>
+      <c r="C20" s="18" t="n">
+        <v>20.9</v>
+      </c>
+      <c r="D20" s="18" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="E20" s="18" t="n">
+        <v>8.7</v>
+      </c>
+      <c r="F20" s="18" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="G20" s="18" t="n">
+        <v>59.6</v>
+      </c>
+      <c r="H20" s="19" t="n">
+        <v>10.1</v>
+      </c>
+      <c r="K20" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="L20" s="43" t="n">
+        <v>12</v>
+      </c>
+      <c r="M20" s="44" t="n">
+        <f aca="false">IF(L20 = "",,(L20-$L$26))</f>
+        <v>5.5</v>
+      </c>
+      <c r="N20" s="44" t="n">
+        <f aca="false">IF(L20 = "",,POWER((L20-$L$26),2))</f>
+        <v>30.25</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="10"/>
+      <c r="B21" s="23" t="n">
+        <v>3</v>
+      </c>
+      <c r="C21" s="24" t="n">
+        <v>18</v>
+      </c>
+      <c r="D21" s="24" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E21" s="24" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="F21" s="24" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="G21" s="24" t="n">
+        <v>71.5</v>
+      </c>
+      <c r="H21" s="25" t="n">
+        <v>16.3</v>
+      </c>
+      <c r="K21" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="L21" s="43" t="n">
+        <v>2</v>
+      </c>
+      <c r="M21" s="44" t="n">
+        <f aca="false">IF(L21 = "",,(L21-$L$26))</f>
+        <v>-4.5</v>
+      </c>
+      <c r="N21" s="44" t="n">
+        <f aca="false">IF(L21 = "",,POWER((L21-$L$26),2))</f>
+        <v>20.25</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="10"/>
+      <c r="B22" s="17" t="n">
+        <v>4</v>
+      </c>
+      <c r="C22" s="18" t="n">
+        <v>15.7</v>
+      </c>
+      <c r="D22" s="18" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="E22" s="18" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="F22" s="18" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="G22" s="18" t="n">
+        <v>78.7</v>
+      </c>
+      <c r="H22" s="19" t="n">
+        <v>10.9</v>
+      </c>
+      <c r="K22" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="L22" s="43" t="n">
+        <v>3</v>
+      </c>
+      <c r="M22" s="44" t="n">
+        <f aca="false">IF(L22 = "",,(L22-$L$26))</f>
+        <v>-3.5</v>
+      </c>
+      <c r="N22" s="44" t="n">
+        <f aca="false">IF(L22 = "",,POWER((L22-$L$26),2))</f>
+        <v>12.25</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="10"/>
+      <c r="B23" s="23" t="n">
+        <v>5</v>
+      </c>
+      <c r="C23" s="24" t="n">
+        <v>14.5</v>
+      </c>
+      <c r="D23" s="24" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E23" s="24" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="F23" s="24" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="G23" s="24" t="n">
+        <v>84.4</v>
+      </c>
+      <c r="H23" s="25" t="n">
+        <v>10.8</v>
+      </c>
+      <c r="K23" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="L23" s="43" t="n">
+        <v>8</v>
+      </c>
+      <c r="M23" s="44" t="n">
+        <f aca="false">IF(L23 = "",,(L23-$L$26))</f>
+        <v>1.5</v>
+      </c>
+      <c r="N23" s="44" t="n">
+        <f aca="false">IF(L23 = "",,POWER((L23-$L$26),2))</f>
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="10"/>
+      <c r="B24" s="17" t="n">
+        <v>6</v>
+      </c>
+      <c r="C24" s="18" t="n">
+        <v>14.9</v>
+      </c>
+      <c r="D24" s="18" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="E24" s="18" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="F24" s="18" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="G24" s="18" t="n">
+        <v>83.2</v>
+      </c>
+      <c r="H24" s="19" t="n">
+        <v>12.1</v>
+      </c>
+      <c r="K24" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="L24" s="43" t="n">
+        <v>5</v>
+      </c>
+      <c r="M24" s="44" t="n">
+        <f aca="false">IF(L24 = "",,(L24-$L$26))</f>
+        <v>-1.5</v>
+      </c>
+      <c r="N24" s="44" t="n">
+        <f aca="false">IF(L24 = "",,POWER((L24-$L$26),2))</f>
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="10"/>
+      <c r="B25" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="33" t="n">
+        <v>18.6</v>
+      </c>
+      <c r="D25" s="33" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="E25" s="33" t="n">
+        <v>5</v>
+      </c>
+      <c r="F25" s="33" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="G25" s="33" t="n">
+        <v>73.9</v>
+      </c>
+      <c r="H25" s="34" t="n">
+        <v>10.9</v>
+      </c>
+      <c r="K25" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="L25" s="43" t="n">
+        <v>7</v>
+      </c>
+      <c r="M25" s="44" t="n">
+        <f aca="false">IF(L25 = "",,(L25-$L$26))</f>
+        <v>0.5</v>
+      </c>
+      <c r="N25" s="44" t="n">
+        <f aca="false">IF(L25 = "",,POWER((L25-$L$26),2))</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="35"/>
+      <c r="B26" s="35"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="36"/>
+      <c r="H26" s="36"/>
+      <c r="K26" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="L26" s="46" t="n">
+        <f aca="false">AVERAGE(L16:L25)</f>
+        <v>6.5</v>
+      </c>
+      <c r="M26" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="N26" s="46" t="n">
+        <f aca="false">SUM(N16:N25)</f>
+        <v>88.5</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="C27" s="38" t="n">
+        <v>26</v>
+      </c>
+      <c r="D27" s="38" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="E27" s="38" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="F27" s="38" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="G27" s="38" t="n">
+        <v>65.3</v>
+      </c>
+      <c r="H27" s="39" t="n">
+        <v>13.4</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="10"/>
+      <c r="B28" s="23" t="n">
+        <v>2</v>
+      </c>
+      <c r="C28" s="24" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="D28" s="24" t="n">
+        <v>5</v>
+      </c>
+      <c r="E28" s="24" t="n">
+        <v>12.8</v>
+      </c>
+      <c r="F28" s="24" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="G28" s="24" t="n">
+        <v>50.8</v>
+      </c>
+      <c r="H28" s="25" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="K28" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="L28" s="47" t="n">
+        <f aca="false">SQRT((N26/COUNTIF(L16:L25,"&lt;&gt;")))</f>
+        <v>2.9748949561287</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="10"/>
+      <c r="B29" s="17" t="n">
+        <v>3</v>
+      </c>
+      <c r="C29" s="18" t="n">
+        <v>16.3</v>
+      </c>
+      <c r="D29" s="18" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="E29" s="18" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="F29" s="18" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="G29" s="18" t="n">
+        <v>75.7</v>
+      </c>
+      <c r="H29" s="19" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="10"/>
+      <c r="B30" s="23" t="n">
+        <v>4</v>
+      </c>
+      <c r="C30" s="24" t="n">
+        <v>15.4</v>
+      </c>
+      <c r="D30" s="24" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="E30" s="24" t="n">
+        <v>3</v>
+      </c>
+      <c r="F30" s="24" t="n">
+        <v>3</v>
+      </c>
+      <c r="G30" s="24" t="n">
+        <v>82.7</v>
+      </c>
+      <c r="H30" s="25" t="n">
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="10"/>
+      <c r="B31" s="17" t="n">
+        <v>5</v>
+      </c>
+      <c r="C31" s="18" t="n">
+        <v>14.5</v>
+      </c>
+      <c r="D31" s="18" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="E31" s="18" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="F31" s="18" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="G31" s="18" t="n">
+        <v>84.9</v>
+      </c>
+      <c r="H31" s="19" t="n">
+        <v>11.8</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="10"/>
+      <c r="B32" s="23" t="n">
+        <v>6</v>
+      </c>
+      <c r="C32" s="24" t="n">
+        <v>15.1</v>
+      </c>
+      <c r="D32" s="24" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E32" s="24" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="F32" s="24" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="G32" s="24" t="n">
+        <v>82.7</v>
+      </c>
+      <c r="H32" s="25" t="n">
+        <v>13.4</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="10"/>
+      <c r="B33" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" s="41" t="n">
+        <v>18.8</v>
+      </c>
+      <c r="D33" s="41" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="E33" s="41" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="F33" s="41" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="G33" s="41" t="n">
+        <v>73.6</v>
+      </c>
+      <c r="H33" s="42" t="n">
+        <v>8.3</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="35"/>
+      <c r="B34" s="35"/>
+      <c r="C34" s="36"/>
+      <c r="D34" s="36"/>
+      <c r="E34" s="36"/>
+      <c r="F34" s="36"/>
+      <c r="G34" s="36"/>
+      <c r="H34" s="36"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C35" s="12" t="n">
+        <v>33.8</v>
+      </c>
+      <c r="D35" s="12" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="E35" s="12" t="n">
+        <v>11.9</v>
+      </c>
+      <c r="F35" s="12" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="G35" s="12" t="n">
+        <v>52.5</v>
+      </c>
+      <c r="H35" s="13" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="10"/>
+      <c r="B36" s="17" t="n">
+        <v>2</v>
+      </c>
+      <c r="C36" s="18" t="n">
+        <v>26.8</v>
+      </c>
+      <c r="D36" s="18" t="n">
+        <v>7.7</v>
+      </c>
+      <c r="E36" s="18" t="n">
+        <v>13.5</v>
+      </c>
+      <c r="F36" s="18" t="n">
+        <v>7.1</v>
+      </c>
+      <c r="G36" s="18" t="n">
+        <v>50.5</v>
+      </c>
+      <c r="H36" s="19" t="n">
+        <v>13.1</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="10"/>
+      <c r="B37" s="23" t="n">
+        <v>3</v>
+      </c>
+      <c r="C37" s="24" t="n">
+        <v>22.2</v>
+      </c>
+      <c r="D37" s="24" t="n">
+        <v>6.8</v>
+      </c>
+      <c r="E37" s="24" t="n">
+        <v>9.1</v>
+      </c>
+      <c r="F37" s="24" t="n">
+        <v>6.4</v>
+      </c>
+      <c r="G37" s="24" t="n">
+        <v>61.3</v>
+      </c>
+      <c r="H37" s="25" t="n">
+        <v>15.9</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="10"/>
+      <c r="B38" s="17" t="n">
+        <v>4</v>
+      </c>
+      <c r="C38" s="18" t="n">
+        <v>21.4</v>
+      </c>
+      <c r="D38" s="18" t="n">
+        <v>9.4</v>
+      </c>
+      <c r="E38" s="18" t="n">
+        <v>8.8</v>
+      </c>
+      <c r="F38" s="18" t="n">
+        <v>9.2</v>
+      </c>
+      <c r="G38" s="18" t="n">
+        <v>64.8</v>
+      </c>
+      <c r="H38" s="19" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="10"/>
+      <c r="B39" s="23" t="n">
+        <v>5</v>
+      </c>
+      <c r="C39" s="24" t="n">
+        <v>19.5</v>
+      </c>
+      <c r="D39" s="24" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="E39" s="24" t="n">
+        <v>7</v>
+      </c>
+      <c r="F39" s="24" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="G39" s="24" t="n">
+        <v>68.5</v>
+      </c>
+      <c r="H39" s="25" t="n">
+        <v>17.6</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="10"/>
+      <c r="B40" s="17" t="n">
+        <v>6</v>
+      </c>
+      <c r="C40" s="18" t="n">
+        <v>18.1</v>
+      </c>
+      <c r="D40" s="18" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="E40" s="18" t="n">
+        <v>5.8</v>
+      </c>
+      <c r="F40" s="18" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="G40" s="18" t="n">
+        <v>71.5</v>
+      </c>
+      <c r="H40" s="19" t="n">
+        <v>16.6</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="10"/>
+      <c r="B41" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" s="33" t="n">
+        <v>23.6</v>
+      </c>
+      <c r="D41" s="33" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="E41" s="33" t="n">
+        <v>9.4</v>
+      </c>
+      <c r="F41" s="33" t="n">
+        <v>5.2</v>
+      </c>
+      <c r="G41" s="33" t="n">
+        <v>61.4</v>
+      </c>
+      <c r="H41" s="34" t="n">
+        <v>12.9</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="35"/>
+      <c r="B42" s="35"/>
+      <c r="C42" s="36"/>
+      <c r="D42" s="36"/>
+      <c r="E42" s="36"/>
+      <c r="F42" s="36"/>
+      <c r="G42" s="36"/>
+      <c r="H42" s="36"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="10" t="n">
+        <v>70</v>
+      </c>
+      <c r="B43" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="C43" s="38" t="n">
+        <v>33.4</v>
+      </c>
+      <c r="D43" s="38" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="E43" s="38" t="n">
+        <v>11.9</v>
+      </c>
+      <c r="F43" s="38" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="G43" s="38" t="n">
+        <v>52.4</v>
+      </c>
+      <c r="H43" s="39" t="n">
+        <v>10.3</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="10"/>
+      <c r="B44" s="23" t="n">
+        <v>2</v>
+      </c>
+      <c r="C44" s="24" t="n">
+        <v>24.1</v>
+      </c>
+      <c r="D44" s="24" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="E44" s="24" t="n">
+        <v>11.6</v>
+      </c>
+      <c r="F44" s="24" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="G44" s="24" t="n">
+        <v>53.2</v>
+      </c>
+      <c r="H44" s="25" t="n">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="10"/>
+      <c r="B45" s="17" t="n">
+        <v>3</v>
+      </c>
+      <c r="C45" s="18" t="n">
+        <v>22</v>
+      </c>
+      <c r="D45" s="18" t="n">
+        <v>7.9</v>
+      </c>
+      <c r="E45" s="18" t="n">
+        <v>9.9</v>
+      </c>
+      <c r="F45" s="18" t="n">
+        <v>7.9</v>
+      </c>
+      <c r="G45" s="18" t="n">
+        <v>59.3</v>
+      </c>
+      <c r="H45" s="19" t="n">
+        <v>13.8</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="10"/>
+      <c r="B46" s="23" t="n">
+        <v>4</v>
+      </c>
+      <c r="C46" s="24" t="n">
+        <v>17.9</v>
+      </c>
+      <c r="D46" s="24" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="E46" s="24" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="F46" s="24" t="n">
+        <v>4</v>
+      </c>
+      <c r="G46" s="24" t="n">
+        <v>71.5</v>
+      </c>
+      <c r="H46" s="25" t="n">
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="10"/>
+      <c r="B47" s="17" t="n">
+        <v>5</v>
+      </c>
+      <c r="C47" s="18" t="n">
+        <v>18.5</v>
+      </c>
+      <c r="D47" s="18" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="E47" s="18" t="n">
+        <v>5.8</v>
+      </c>
+      <c r="F47" s="18" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="G47" s="18" t="n">
+        <v>72</v>
+      </c>
+      <c r="H47" s="19" t="n">
+        <v>16.7</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="10"/>
+      <c r="B48" s="23" t="n">
+        <v>6</v>
+      </c>
+      <c r="C48" s="24" t="n">
+        <v>17.8</v>
+      </c>
+      <c r="D48" s="24" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="E48" s="24" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="F48" s="24" t="n">
+        <v>5.2</v>
+      </c>
+      <c r="G48" s="24" t="n">
+        <v>73.8</v>
+      </c>
+      <c r="H48" s="25" t="n">
+        <v>18.4</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="10"/>
+      <c r="B49" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="C49" s="41" t="n">
+        <v>22.5</v>
+      </c>
+      <c r="D49" s="41" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="E49" s="41" t="n">
+        <v>8.3</v>
+      </c>
+      <c r="F49" s="41" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="G49" s="41" t="n">
+        <v>63.7</v>
+      </c>
+      <c r="H49" s="42" t="n">
+        <v>10.9</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="A3:A9"/>
+    <mergeCell ref="A11:A17"/>
+    <mergeCell ref="A19:A25"/>
+    <mergeCell ref="A27:A33"/>
+    <mergeCell ref="A35:A41"/>
+    <mergeCell ref="A43:A49"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>